<commit_message>
20211103 CRE21-017	To include number of reimbursed transactions by school in the season for reports eHS(S)D0032 and eHS(S)D0033
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSD0032-PPP Claim_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSD0032-PPP Claim_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-017 (PPP report add reimbursed tx)\Front-end\ExcelGenerator\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="930" yWindow="1290" windowWidth="18570" windowHeight="7500" tabRatio="760"/>
   </bookViews>
@@ -15,12 +20,12 @@
     <sheet name="Remark" sheetId="6" r:id="rId6"/>
     <sheet name="Change History" sheetId="25" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="90">
   <si>
     <t/>
   </si>
@@ -333,16 +338,28 @@
   </si>
   <si>
     <t>CRE19-001</t>
+  </si>
+  <si>
+    <t>No. of Reimbursed Transactions</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>To include number of reimbursed transactions by school in the season for reports eHS(S)D0032 and eHS(S)D0033</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE21-017</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+    <numFmt numFmtId="178" formatCode="0_ "/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -494,7 +511,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -506,13 +523,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -521,22 +538,22 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -545,22 +562,22 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -572,7 +589,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -719,7 +736,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,7 +763,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -836,7 +853,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -871,7 +888,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2259,7 +2276,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2267,33 +2284,37 @@
   <cols>
     <col min="1" max="1" width="18.625" style="43"/>
     <col min="2" max="6" width="18.625" style="93"/>
-    <col min="7" max="16384" width="18.625" style="72"/>
+    <col min="7" max="7" width="33.375" style="93" customWidth="1"/>
+    <col min="8" max="16384" width="18.625" style="72"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="str">
         <f>Content!A4 &amp; ": " &amp;Content!B4</f>
         <v>eHS(S)D0032-03: Report on yearly PPP-PS claim transaction by school code (YYYY/YY)</v>
       </c>
       <c r="B1" s="92"/>
       <c r="F1" s="94"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="94"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
       <c r="B2" s="92"/>
       <c r="F2" s="94"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="94"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="92"/>
       <c r="F3" s="94"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="94"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="82"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="98" t="s">
         <v>74</v>
       </c>
@@ -2312,8 +2333,11 @@
       <c r="F5" s="96" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="96" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="82"/>
     </row>
   </sheetData>
@@ -2679,7 +2703,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2748,6 +2772,20 @@
         <v>43747</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="89">
+        <v>3</v>
+      </c>
+      <c r="B6" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="104" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="90">
+        <v>44503</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>